<commit_message>
Comparison of name of delivery mechanism should be case-insensitive
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_valid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_valid.xlsx
@@ -58,7 +58,7 @@
     <t>Agata Kowalska</t>
   </si>
   <si>
-    <t>Pre-paid card</t>
+    <t>deposit to card</t>
   </si>
   <si>
     <t>Roberts LLC</t>
@@ -79,7 +79,7 @@
     <t>Jan Romaniak</t>
   </si>
   <si>
-    <t>Cash by FSP</t>
+    <t>Referral</t>
   </si>
   <si>
     <t>White-Mcgrath</t>
@@ -107,7 +107,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -132,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -215,13 +215,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -253,6 +349,36 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1367,7 +1493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1487,6 +1613,97 @@
       </c>
       <c r="K3" s="10"/>
     </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>